<commit_message>
Corrected the indices for the dubosson data
</commit_message>
<xml_diff>
--- a/data/manual_calculations.xlsx
+++ b/data/manual_calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Irina/Google Drive/MacLaptop/Research/github/mage_algorithm_data/graphics_scripts/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\njfer\OneDrive\Documents\Documents Backup\TAMU\Research - Dr. Gaynanova\iglu\Official MAGE Data Repo\mage_algorithm_data\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C2B15B-B822-294F-A560-51D88386DCF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3962A4C4-6FF1-4650-AAB9-A2FAF413FC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20720" windowHeight="13280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4030" yWindow="1000" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -477,14 +477,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="8.6640625" style="1"/>
+    <col min="4" max="4" width="8.6328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -516,7 +518,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -524,7 +526,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="5">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" s="6">
         <v>52</v>
@@ -545,15 +547,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="5">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="5">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="D3" s="6">
         <v>118</v>
@@ -574,15 +576,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="5">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C4" s="5">
-        <v>645</v>
+        <v>634</v>
       </c>
       <c r="D4" s="6">
         <v>264</v>
@@ -603,15 +605,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="5">
-        <v>646</v>
+        <v>635</v>
       </c>
       <c r="C5" s="5">
-        <v>939</v>
+        <v>923</v>
       </c>
       <c r="D5" s="6">
         <v>183</v>
@@ -632,15 +634,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="5">
-        <v>940</v>
+        <v>924</v>
       </c>
       <c r="C6" s="5">
-        <v>1233</v>
+        <v>1211</v>
       </c>
       <c r="D6" s="6">
         <v>150</v>
@@ -661,15 +663,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="5">
-        <v>1497</v>
+        <v>1470</v>
       </c>
       <c r="C7" s="5">
-        <v>1787</v>
+        <v>1757</v>
       </c>
       <c r="D7" s="6">
         <v>266</v>
@@ -690,15 +692,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="5">
-        <v>1788</v>
+        <v>1758</v>
       </c>
       <c r="C8" s="5">
-        <v>2078</v>
+        <v>2045</v>
       </c>
       <c r="D8" s="6">
         <v>166</v>
@@ -717,7 +719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
@@ -746,7 +748,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
@@ -775,7 +777,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -804,7 +806,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
@@ -833,7 +835,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
@@ -865,7 +867,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
@@ -894,7 +896,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
@@ -923,7 +925,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>9</v>
       </c>
@@ -955,7 +957,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>9</v>
       </c>
@@ -984,7 +986,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>9</v>
       </c>
@@ -1013,7 +1015,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>9</v>
       </c>
@@ -1045,7 +1047,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>9</v>
       </c>
@@ -1077,7 +1079,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>9</v>
       </c>
@@ -1109,7 +1111,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>9</v>
       </c>
@@ -1141,7 +1143,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>9</v>
       </c>
@@ -1173,7 +1175,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>9</v>
       </c>
@@ -1205,7 +1207,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>12</v>
       </c>
@@ -1234,7 +1236,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>12</v>
       </c>
@@ -1263,7 +1265,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>12</v>
       </c>
@@ -1292,7 +1294,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>12</v>
       </c>
@@ -1321,7 +1323,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>12</v>
       </c>
@@ -1350,7 +1352,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>12</v>
       </c>
@@ -1379,7 +1381,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>12</v>
       </c>
@@ -1411,7 +1413,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>12</v>
       </c>
@@ -1440,7 +1442,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>12</v>
       </c>
@@ -1469,7 +1471,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>12</v>
       </c>
@@ -1498,7 +1500,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>12</v>
       </c>
@@ -1527,7 +1529,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>12</v>
       </c>
@@ -1556,7 +1558,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>12</v>
       </c>
@@ -1588,7 +1590,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>12</v>
       </c>
@@ -1617,7 +1619,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>12</v>
       </c>
@@ -1646,7 +1648,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>12</v>
       </c>
@@ -1675,7 +1677,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>12</v>
       </c>
@@ -1704,7 +1706,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>12</v>
       </c>
@@ -1733,7 +1735,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>19</v>
       </c>
@@ -1762,7 +1764,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>19</v>
       </c>
@@ -1791,7 +1793,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>19</v>
       </c>
@@ -1820,7 +1822,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>19</v>
       </c>
@@ -1852,7 +1854,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>19</v>
       </c>
@@ -1881,7 +1883,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>19</v>
       </c>
@@ -1911,7 +1913,7 @@
       </c>
       <c r="J48" s="7"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>19</v>
       </c>
@@ -1940,7 +1942,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>19</v>
       </c>
@@ -1969,7 +1971,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>19</v>
       </c>
@@ -1998,7 +2000,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
moved plot_scripts -> data to decrease ambiguity. Plot_scripts was just plotting the raw CGM data so it should go with the raw data
</commit_message>
<xml_diff>
--- a/data/manual_calculations.xlsx
+++ b/data/manual_calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\njfer\OneDrive\Documents\Documents Backup\TAMU\Research - Dr. Gaynanova\iglu\Official MAGE Data Repo\mage_algorithm_data\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathanielfernandes/Documents/Projects/mage_algorithm_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3962A4C4-6FF1-4650-AAB9-A2FAF413FC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB99CDA8-1A8A-EE40-9044-6C254BFA0331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4030" yWindow="1000" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="35">
   <si>
     <t>start</t>
   </si>
@@ -115,6 +115,21 @@
   </si>
   <si>
     <t>dataset</t>
+  </si>
+  <si>
+    <t>Dubosson2018_processed.csv</t>
+  </si>
+  <si>
+    <t>Hall2018_processed.csv</t>
+  </si>
+  <si>
+    <t>Tsalikian2005_processed.csv</t>
+  </si>
+  <si>
+    <t>ExampleData5Subjects.csv</t>
+  </si>
+  <si>
+    <t>dataset_filename</t>
   </si>
 </sst>
 </file>
@@ -182,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -195,6 +210,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,67 +491,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="8.6328125" style="1"/>
+    <col min="5" max="5" width="8.6640625" style="1"/>
+    <col min="11" max="11" width="8.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5">
-        <v>1</v>
+      <c r="B2" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="C2" s="5">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5">
         <v>58</v>
       </c>
-      <c r="D2" s="6">
+      <c r="E2" s="6">
         <v>52</v>
       </c>
-      <c r="E2" s="5">
-        <v>0</v>
-      </c>
       <c r="F2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="5">
         <v>1</v>
@@ -546,28 +566,31 @@
       <c r="I2" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="5">
         <v>59</v>
       </c>
-      <c r="C3" s="5">
+      <c r="D3" s="5">
         <v>346</v>
       </c>
-      <c r="D3" s="6">
+      <c r="E3" s="6">
         <v>118</v>
       </c>
-      <c r="E3" s="5">
-        <v>0</v>
-      </c>
       <c r="F3" s="5">
         <v>0</v>
       </c>
       <c r="G3" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="5">
         <v>1</v>
@@ -575,28 +598,31 @@
       <c r="I3" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="5">
         <v>347</v>
       </c>
-      <c r="C4" s="5">
+      <c r="D4" s="5">
         <v>634</v>
       </c>
-      <c r="D4" s="6">
+      <c r="E4" s="6">
         <v>264</v>
       </c>
-      <c r="E4" s="5">
-        <v>0</v>
-      </c>
       <c r="F4" s="5">
         <v>0</v>
       </c>
       <c r="G4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="5">
         <v>1</v>
@@ -604,28 +630,31 @@
       <c r="I4" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="5">
         <v>635</v>
       </c>
-      <c r="C5" s="5">
+      <c r="D5" s="5">
         <v>923</v>
       </c>
-      <c r="D5" s="6">
+      <c r="E5" s="6">
         <v>183</v>
       </c>
-      <c r="E5" s="5">
-        <v>0</v>
-      </c>
       <c r="F5" s="5">
         <v>0</v>
       </c>
       <c r="G5" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="5">
         <v>1</v>
@@ -633,28 +662,31 @@
       <c r="I5" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="5">
         <v>924</v>
       </c>
-      <c r="C6" s="5">
+      <c r="D6" s="5">
         <v>1211</v>
       </c>
-      <c r="D6" s="6">
+      <c r="E6" s="6">
         <v>150</v>
       </c>
-      <c r="E6" s="5">
-        <v>0</v>
-      </c>
       <c r="F6" s="5">
         <v>0</v>
       </c>
       <c r="G6" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="5">
         <v>1</v>
@@ -662,1370 +694,1510 @@
       <c r="I6" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J6" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="5">
         <v>1470</v>
       </c>
-      <c r="C7" s="5">
+      <c r="D7" s="5">
         <v>1757</v>
       </c>
-      <c r="D7" s="6">
+      <c r="E7" s="6">
         <v>266</v>
       </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
       <c r="F7" s="5">
         <v>0</v>
       </c>
       <c r="G7" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="5">
         <v>1</v>
       </c>
       <c r="I7" s="5">
+        <v>1</v>
+      </c>
+      <c r="J7" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="5">
         <v>1758</v>
       </c>
-      <c r="C8" s="5">
+      <c r="D8" s="5">
         <v>2045</v>
       </c>
-      <c r="D8" s="6">
+      <c r="E8" s="6">
         <v>166</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5">
-        <v>0</v>
-      </c>
+      <c r="F8" s="5"/>
       <c r="G8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" s="5">
         <v>1</v>
       </c>
       <c r="I8" s="5">
+        <v>1</v>
+      </c>
+      <c r="J8" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5">
-        <v>1</v>
+      <c r="B9" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
         <v>244</v>
       </c>
-      <c r="D9" s="11">
+      <c r="E9" s="11">
         <v>31</v>
       </c>
-      <c r="E9" s="5">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9" s="5">
-        <v>1</v>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
       </c>
       <c r="H9" s="5">
-        <v>0</v>
-      </c>
-      <c r="I9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="5">
         <v>245</v>
       </c>
-      <c r="C10" s="5">
+      <c r="D10" s="5">
         <v>531</v>
       </c>
-      <c r="D10" s="6">
+      <c r="E10" s="6">
         <v>107</v>
       </c>
-      <c r="E10" s="5">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10" s="5">
-        <v>1</v>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
       </c>
       <c r="H10" s="5">
-        <v>0</v>
-      </c>
-      <c r="I10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="5">
         <v>532</v>
       </c>
-      <c r="C11" s="5">
+      <c r="D11" s="5">
         <v>754</v>
       </c>
-      <c r="D11" s="6">
+      <c r="E11" s="6">
         <v>83</v>
       </c>
-      <c r="E11" s="5">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11" s="5">
-        <v>1</v>
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
       </c>
       <c r="H11" s="5">
-        <v>0</v>
-      </c>
-      <c r="I11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="5">
         <v>755</v>
       </c>
-      <c r="C12" s="5">
+      <c r="D12" s="5">
         <v>849</v>
       </c>
-      <c r="D12" s="6">
+      <c r="E12" s="6">
         <v>91</v>
       </c>
-      <c r="E12" s="5">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12" s="5">
-        <v>1</v>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
       </c>
       <c r="H12" s="5">
-        <v>0</v>
-      </c>
-      <c r="I12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="5">
         <v>849</v>
       </c>
-      <c r="C13" s="5">
+      <c r="D13" s="5">
         <v>1101</v>
       </c>
-      <c r="D13" s="6">
+      <c r="E13" s="6">
         <v>58</v>
       </c>
-      <c r="E13" s="8">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13" s="5">
-        <v>1</v>
+      <c r="F13" s="8">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
       </c>
       <c r="H13" s="5">
-        <v>0</v>
-      </c>
-      <c r="I13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="5">
         <v>1102</v>
       </c>
-      <c r="C14" s="5">
+      <c r="D14" s="5">
         <v>1379</v>
       </c>
-      <c r="D14" s="6">
+      <c r="E14" s="6">
         <v>51</v>
       </c>
-      <c r="E14" s="5">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14" s="5">
-        <v>1</v>
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
       </c>
       <c r="H14" s="5">
-        <v>0</v>
-      </c>
-      <c r="I14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="5">
+        <v>0</v>
+      </c>
+      <c r="J14" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="5">
         <v>1380</v>
       </c>
-      <c r="C15" s="5">
+      <c r="D15" s="5">
         <v>1666</v>
       </c>
-      <c r="D15" s="6">
+      <c r="E15" s="6">
         <v>57</v>
       </c>
-      <c r="E15" s="5">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15" s="5">
-        <v>1</v>
+      <c r="F15" s="5">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
       </c>
       <c r="H15" s="5">
-        <v>0</v>
-      </c>
-      <c r="I15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="5">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="5">
         <v>1667</v>
       </c>
-      <c r="C16" s="5">
+      <c r="D16" s="5">
         <v>1846</v>
       </c>
-      <c r="D16" s="6">
+      <c r="E16" s="6">
         <v>34</v>
       </c>
-      <c r="E16" s="8">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16" s="5">
-        <v>1</v>
+      <c r="F16" s="8">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
       </c>
       <c r="H16" s="5">
-        <v>0</v>
-      </c>
-      <c r="I16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="5">
         <v>1847</v>
       </c>
-      <c r="C17" s="5">
+      <c r="D17" s="5">
         <v>2124</v>
       </c>
-      <c r="D17" s="6">
+      <c r="E17" s="6">
         <v>53</v>
       </c>
-      <c r="E17" s="5">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17" s="5">
-        <v>1</v>
+      <c r="F17" s="5">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
       </c>
       <c r="H17" s="5">
-        <v>0</v>
-      </c>
-      <c r="I17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="5">
+        <v>0</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="5">
         <v>2125</v>
       </c>
-      <c r="C18" s="5">
+      <c r="D18" s="5">
         <v>2303</v>
       </c>
-      <c r="D18" s="6">
+      <c r="E18" s="6">
         <v>65</v>
       </c>
-      <c r="E18" s="5">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18" s="5">
-        <v>1</v>
+      <c r="F18" s="5">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
       </c>
       <c r="H18" s="5">
-        <v>0</v>
-      </c>
-      <c r="I18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="5">
         <v>2304</v>
       </c>
-      <c r="C19" s="5">
+      <c r="D19" s="5">
         <v>2585</v>
       </c>
-      <c r="D19" s="6">
+      <c r="E19" s="6">
         <v>47</v>
       </c>
-      <c r="E19" s="8">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19" s="5">
-        <v>1</v>
+      <c r="F19" s="8">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
       </c>
       <c r="H19" s="5">
-        <v>0</v>
-      </c>
-      <c r="I19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="5">
+        <v>0</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="3">
         <v>7697</v>
       </c>
-      <c r="C20" s="3">
+      <c r="D20" s="3">
         <v>7953</v>
       </c>
-      <c r="D20" s="4">
+      <c r="E20" s="4">
         <v>52</v>
       </c>
-      <c r="E20" s="3">
-        <v>1</v>
-      </c>
       <c r="F20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" s="3">
-        <v>0</v>
-      </c>
-      <c r="I20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0</v>
+      </c>
+      <c r="J20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="K20" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="3">
         <v>7954</v>
       </c>
-      <c r="C21" s="3">
+      <c r="D21" s="3">
         <v>8128</v>
       </c>
-      <c r="D21" s="4">
+      <c r="E21" s="4">
         <v>75</v>
       </c>
-      <c r="E21" s="3">
-        <v>1</v>
-      </c>
       <c r="F21" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" s="3">
-        <v>0</v>
-      </c>
-      <c r="I21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="3">
+        <v>0</v>
+      </c>
+      <c r="J21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="K21" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="3">
         <v>8129</v>
       </c>
-      <c r="C22" s="3">
+      <c r="D22" s="3">
         <v>8343</v>
       </c>
-      <c r="D22" s="4">
+      <c r="E22" s="4">
         <v>46</v>
       </c>
-      <c r="E22" s="3">
-        <v>1</v>
-      </c>
       <c r="F22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" s="3">
-        <v>0</v>
-      </c>
-      <c r="I22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0</v>
+      </c>
+      <c r="J22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="K22" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="3">
         <v>8344</v>
       </c>
-      <c r="C23" s="3">
+      <c r="D23" s="3">
         <v>8513</v>
       </c>
-      <c r="D23" s="4">
+      <c r="E23" s="4">
         <v>40</v>
       </c>
-      <c r="E23" s="3">
-        <v>1</v>
-      </c>
       <c r="F23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" s="3">
-        <v>0</v>
-      </c>
-      <c r="I23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0</v>
+      </c>
+      <c r="J23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="K23" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="3">
         <v>8514</v>
       </c>
-      <c r="C24" s="3">
+      <c r="D24" s="3">
         <v>8745</v>
       </c>
-      <c r="D24" s="4">
+      <c r="E24" s="4">
         <v>61</v>
       </c>
-      <c r="E24" s="3">
-        <v>1</v>
-      </c>
       <c r="F24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" s="3">
-        <v>0</v>
-      </c>
-      <c r="I24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0</v>
+      </c>
+      <c r="J24" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="3" t="s">
+      <c r="K24" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="5">
         <v>405</v>
       </c>
-      <c r="C25" s="5">
+      <c r="D25" s="5">
         <v>644</v>
       </c>
-      <c r="D25" s="6">
+      <c r="E25" s="6">
         <v>47</v>
       </c>
-      <c r="E25" s="5">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25" s="5">
-        <v>1</v>
+      <c r="F25" s="5">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
       </c>
       <c r="H25" s="5">
+        <v>1</v>
+      </c>
+      <c r="I25" s="5">
         <v>2</v>
       </c>
-      <c r="I25" s="5" t="s">
+      <c r="J25" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="5">
         <v>2994</v>
       </c>
-      <c r="C26" s="5">
+      <c r="D26" s="5">
         <v>3281</v>
       </c>
-      <c r="D26" s="6">
+      <c r="E26" s="6">
         <v>70</v>
       </c>
-      <c r="E26" s="5">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26" s="5">
-        <v>1</v>
+      <c r="F26" s="5">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
       </c>
       <c r="H26" s="5">
+        <v>1</v>
+      </c>
+      <c r="I26" s="5">
         <v>2</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="J26" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="5">
         <v>3282</v>
       </c>
-      <c r="C27" s="5">
+      <c r="D27" s="5">
         <v>3569</v>
       </c>
-      <c r="D27" s="6">
+      <c r="E27" s="6">
         <v>81</v>
       </c>
-      <c r="E27" s="5">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27" s="5">
-        <v>1</v>
+      <c r="F27" s="5">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
       </c>
       <c r="H27" s="5">
+        <v>1</v>
+      </c>
+      <c r="I27" s="5">
         <v>2</v>
       </c>
-      <c r="I27" s="5" t="s">
+      <c r="J27" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="5">
         <v>3570</v>
       </c>
-      <c r="C28" s="5">
+      <c r="D28" s="5">
         <v>3857</v>
       </c>
-      <c r="D28" s="2">
+      <c r="E28" s="2">
         <v>154</v>
       </c>
-      <c r="E28" s="5">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28" s="5">
-        <v>1</v>
+      <c r="F28" s="5">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
       </c>
       <c r="H28" s="5">
+        <v>1</v>
+      </c>
+      <c r="I28" s="5">
         <v>2</v>
       </c>
-      <c r="I28" s="5" t="s">
+      <c r="J28" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="5">
         <v>3858</v>
       </c>
-      <c r="C29" s="5">
+      <c r="D29" s="5">
         <v>4144</v>
       </c>
-      <c r="D29" s="2">
+      <c r="E29" s="2">
         <v>104</v>
       </c>
-      <c r="E29" s="5">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29" s="5">
-        <v>1</v>
+      <c r="F29" s="5">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
       </c>
       <c r="H29" s="5">
+        <v>1</v>
+      </c>
+      <c r="I29" s="5">
         <v>2</v>
       </c>
-      <c r="I29" s="5" t="s">
+      <c r="J29" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="5">
         <v>4145</v>
       </c>
-      <c r="C30" s="5">
+      <c r="D30" s="5">
         <v>4432</v>
       </c>
-      <c r="D30" s="6">
+      <c r="E30" s="6">
         <v>95</v>
       </c>
-      <c r="E30" s="5">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30" s="5">
-        <v>1</v>
+      <c r="F30" s="5">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
       </c>
       <c r="H30" s="5">
+        <v>1</v>
+      </c>
+      <c r="I30" s="5">
         <v>2</v>
       </c>
-      <c r="I30" s="5" t="s">
+      <c r="J30" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="5">
         <v>5746</v>
       </c>
-      <c r="C31" s="5">
+      <c r="D31" s="5">
         <v>5842</v>
       </c>
-      <c r="D31" s="6">
+      <c r="E31" s="6">
         <v>89</v>
       </c>
-      <c r="E31" s="8">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-      <c r="G31" s="5">
+      <c r="F31" s="8">
+        <v>0</v>
+      </c>
+      <c r="G31">
         <v>1</v>
       </c>
       <c r="H31" s="5">
+        <v>1</v>
+      </c>
+      <c r="I31" s="5">
         <v>2</v>
       </c>
-      <c r="I31" s="5" t="s">
+      <c r="J31" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K31" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="5">
         <v>7413</v>
       </c>
-      <c r="C32" s="5">
+      <c r="D32" s="5">
         <v>7698</v>
       </c>
-      <c r="D32" s="2">
+      <c r="E32" s="2">
         <v>75</v>
       </c>
-      <c r="E32" s="5">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32" s="5">
-        <v>1</v>
+      <c r="F32" s="5">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
       </c>
       <c r="H32" s="5">
+        <v>1</v>
+      </c>
+      <c r="I32" s="5">
         <v>2</v>
       </c>
-      <c r="I32" s="5" t="s">
+      <c r="J32" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="5">
         <v>7699</v>
       </c>
-      <c r="C33" s="5">
+      <c r="D33" s="5">
         <v>7985</v>
       </c>
-      <c r="D33" s="6">
+      <c r="E33" s="6">
         <v>58</v>
       </c>
-      <c r="E33" s="5">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33" s="5">
-        <v>1</v>
+      <c r="F33" s="5">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
       </c>
       <c r="H33" s="5">
+        <v>1</v>
+      </c>
+      <c r="I33" s="5">
         <v>2</v>
       </c>
-      <c r="I33" s="5" t="s">
+      <c r="J33" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="5">
         <v>7986</v>
       </c>
-      <c r="C34" s="5">
+      <c r="D34" s="5">
         <v>8273</v>
       </c>
-      <c r="D34" s="2">
+      <c r="E34" s="2">
         <v>45</v>
       </c>
-      <c r="E34" s="5">
-        <v>0</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34" s="5">
-        <v>1</v>
+      <c r="F34" s="5">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
       </c>
       <c r="H34" s="5">
+        <v>1</v>
+      </c>
+      <c r="I34" s="5">
         <v>2</v>
       </c>
-      <c r="I34" s="5" t="s">
+      <c r="J34" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="5">
         <v>8274</v>
       </c>
-      <c r="C35" s="5">
+      <c r="D35" s="5">
         <v>8561</v>
       </c>
-      <c r="D35" s="2">
+      <c r="E35" s="2">
         <v>69</v>
       </c>
-      <c r="E35" s="5">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35" s="5">
-        <v>1</v>
+      <c r="F35" s="5">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
       </c>
       <c r="H35" s="5">
+        <v>1</v>
+      </c>
+      <c r="I35" s="5">
         <v>2</v>
       </c>
-      <c r="I35" s="5" t="s">
+      <c r="J35" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="5">
         <v>8562</v>
       </c>
-      <c r="C36" s="5">
+      <c r="D36" s="5">
         <v>8849</v>
       </c>
-      <c r="D36" s="6">
+      <c r="E36" s="6">
         <v>32</v>
       </c>
-      <c r="E36" s="5">
-        <v>0</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="G36" s="5">
-        <v>1</v>
+      <c r="F36" s="5">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
       </c>
       <c r="H36" s="5">
+        <v>1</v>
+      </c>
+      <c r="I36" s="5">
         <v>2</v>
       </c>
-      <c r="I36" s="5" t="s">
+      <c r="J36" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="5">
         <v>11018</v>
       </c>
-      <c r="C37" s="5">
+      <c r="D37" s="5">
         <v>11301</v>
       </c>
-      <c r="D37" s="6">
+      <c r="E37" s="6">
         <v>120</v>
       </c>
-      <c r="E37" s="8">
-        <v>0</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37" s="5">
-        <v>1</v>
+      <c r="F37" s="8">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
       </c>
       <c r="H37" s="5">
+        <v>1</v>
+      </c>
+      <c r="I37" s="5">
         <v>2</v>
       </c>
-      <c r="I37" s="5" t="s">
+      <c r="J37" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J37" t="s">
+      <c r="K37" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="5">
         <v>11302</v>
       </c>
-      <c r="C38" s="5">
+      <c r="D38" s="5">
         <v>11588</v>
       </c>
-      <c r="D38" s="6">
+      <c r="E38" s="6">
         <v>211</v>
       </c>
-      <c r="E38" s="5">
-        <v>0</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38" s="5">
-        <v>1</v>
+      <c r="F38" s="5">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
       </c>
       <c r="H38" s="5">
+        <v>1</v>
+      </c>
+      <c r="I38" s="5">
         <v>2</v>
       </c>
-      <c r="I38" s="5" t="s">
+      <c r="J38" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B39" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="5">
         <v>11589</v>
       </c>
-      <c r="C39" s="5">
+      <c r="D39" s="5">
         <v>11830</v>
       </c>
-      <c r="D39" s="6">
+      <c r="E39" s="6">
         <v>147</v>
       </c>
-      <c r="E39" s="5">
-        <v>1</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39" s="5">
-        <v>1</v>
+      <c r="F39" s="5">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
       </c>
       <c r="H39" s="5">
+        <v>1</v>
+      </c>
+      <c r="I39" s="5">
         <v>2</v>
       </c>
-      <c r="I39" s="5" t="s">
+      <c r="J39" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B40" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="5">
         <v>11831</v>
       </c>
-      <c r="C40" s="5">
+      <c r="D40" s="5">
         <v>12118</v>
       </c>
-      <c r="D40" s="6">
+      <c r="E40" s="6">
         <v>125</v>
       </c>
-      <c r="E40" s="5">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40" s="5">
-        <v>1</v>
+      <c r="F40" s="5">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
       </c>
       <c r="H40" s="5">
+        <v>1</v>
+      </c>
+      <c r="I40" s="5">
         <v>2</v>
       </c>
-      <c r="I40" s="5" t="s">
+      <c r="J40" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B41" s="5">
+      <c r="B41" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="5">
         <v>12119</v>
       </c>
-      <c r="C41" s="5">
+      <c r="D41" s="5">
         <v>12406</v>
       </c>
-      <c r="D41" s="6">
+      <c r="E41" s="6">
         <v>227</v>
       </c>
-      <c r="E41" s="5">
-        <v>0</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41" s="5">
-        <v>1</v>
+      <c r="F41" s="5">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
       </c>
       <c r="H41" s="5">
+        <v>1</v>
+      </c>
+      <c r="I41" s="5">
         <v>2</v>
       </c>
-      <c r="I41" s="5" t="s">
+      <c r="J41" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B42" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="5">
         <v>12653</v>
       </c>
-      <c r="C42" s="5">
+      <c r="D42" s="5">
         <v>12940</v>
       </c>
-      <c r="D42" s="6">
+      <c r="E42" s="6">
         <v>153</v>
       </c>
-      <c r="E42" s="5">
-        <v>0</v>
-      </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-      <c r="G42" s="5">
-        <v>1</v>
+      <c r="F42" s="5">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
       </c>
       <c r="H42" s="5">
+        <v>1</v>
+      </c>
+      <c r="I42" s="5">
         <v>2</v>
       </c>
-      <c r="I42" s="5" t="s">
+      <c r="J42" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B43" s="5">
-        <v>1</v>
+      <c r="B43" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="C43" s="5">
+        <v>1</v>
+      </c>
+      <c r="D43" s="5">
         <v>135</v>
       </c>
-      <c r="D43" s="6">
+      <c r="E43" s="6">
         <v>138</v>
       </c>
-      <c r="E43" s="5">
-        <v>0</v>
-      </c>
-      <c r="F43">
-        <v>1</v>
-      </c>
-      <c r="G43" s="5">
-        <v>0</v>
+      <c r="F43" s="5">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
       </c>
       <c r="H43" s="5">
-        <v>1</v>
-      </c>
-      <c r="I43" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I43" s="5">
+        <v>1</v>
+      </c>
+      <c r="J43" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B44" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" s="5">
         <v>136</v>
       </c>
-      <c r="C44" s="5">
+      <c r="D44" s="5">
         <v>242</v>
       </c>
-      <c r="D44" s="4">
+      <c r="E44" s="4">
         <v>164</v>
       </c>
-      <c r="E44" s="5">
-        <v>0</v>
-      </c>
-      <c r="F44">
-        <v>1</v>
-      </c>
-      <c r="G44" s="5">
-        <v>0</v>
+      <c r="F44" s="5">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
       </c>
       <c r="H44" s="5">
-        <v>1</v>
-      </c>
-      <c r="I44" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I44" s="5">
+        <v>1</v>
+      </c>
+      <c r="J44" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="5">
+      <c r="B45" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45" s="5">
         <v>243</v>
       </c>
-      <c r="C45" s="5">
+      <c r="D45" s="5">
         <v>384</v>
       </c>
-      <c r="D45" s="6">
+      <c r="E45" s="6">
         <v>135</v>
       </c>
-      <c r="E45" s="5">
-        <v>0</v>
-      </c>
-      <c r="F45">
-        <v>1</v>
-      </c>
-      <c r="G45" s="5">
-        <v>0</v>
+      <c r="F45" s="5">
+        <v>0</v>
+      </c>
+      <c r="G45" s="7">
+        <v>1</v>
       </c>
       <c r="H45" s="5">
-        <v>1</v>
-      </c>
-      <c r="I45" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I45" s="5">
+        <v>1</v>
+      </c>
+      <c r="J45" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" s="3">
         <v>385</v>
       </c>
-      <c r="C46" s="3">
+      <c r="D46" s="3">
         <v>455</v>
       </c>
-      <c r="D46" s="4">
+      <c r="E46" s="4">
         <v>15</v>
       </c>
-      <c r="E46" s="3">
-        <v>0</v>
-      </c>
       <c r="F46" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46" s="3">
-        <v>1</v>
-      </c>
-      <c r="I46" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I46" s="3">
+        <v>1</v>
+      </c>
+      <c r="J46" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J46" s="3" t="s">
+      <c r="K46" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B47" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="5">
         <v>456</v>
       </c>
-      <c r="C47" s="5">
+      <c r="D47" s="5">
         <v>561</v>
       </c>
-      <c r="D47" s="6">
+      <c r="E47" s="6">
         <v>45</v>
       </c>
-      <c r="E47" s="5">
-        <v>0</v>
-      </c>
-      <c r="F47">
-        <v>1</v>
-      </c>
-      <c r="G47" s="5">
-        <v>0</v>
+      <c r="F47" s="5">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
       </c>
       <c r="H47" s="5">
-        <v>1</v>
-      </c>
-      <c r="I47" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I47" s="5">
+        <v>1</v>
+      </c>
+      <c r="J47" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B48" s="5">
+      <c r="B48" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" s="5">
         <v>1601</v>
       </c>
-      <c r="C48" s="5">
+      <c r="D48" s="5">
         <v>1755</v>
       </c>
-      <c r="D48" s="6">
+      <c r="E48" s="6">
         <v>55</v>
       </c>
-      <c r="E48" s="5">
-        <v>0</v>
-      </c>
-      <c r="F48">
-        <v>1</v>
-      </c>
-      <c r="G48" s="5">
-        <v>0</v>
+      <c r="F48" s="5">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
       </c>
       <c r="H48" s="5">
-        <v>1</v>
-      </c>
-      <c r="I48" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I48" s="5">
+        <v>1</v>
+      </c>
+      <c r="J48" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J48" s="7"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B49" s="5">
+      <c r="B49" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" s="5">
         <v>3076</v>
       </c>
-      <c r="C49" s="5">
+      <c r="D49" s="5">
         <v>3230</v>
       </c>
-      <c r="D49" s="6">
+      <c r="E49" s="6">
         <v>87</v>
       </c>
-      <c r="E49" s="5">
-        <v>0</v>
-      </c>
-      <c r="F49">
-        <v>1</v>
-      </c>
-      <c r="G49" s="5">
-        <v>0</v>
+      <c r="F49" s="5">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
       </c>
       <c r="H49" s="5">
-        <v>1</v>
-      </c>
-      <c r="I49" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I49" s="5">
+        <v>1</v>
+      </c>
+      <c r="J49" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B50" s="5">
+      <c r="B50" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" s="5">
         <v>3319</v>
       </c>
-      <c r="C50" s="5">
+      <c r="D50" s="5">
         <v>3475</v>
       </c>
-      <c r="D50" s="6">
+      <c r="E50" s="6">
         <v>360</v>
       </c>
-      <c r="E50" s="5">
-        <v>0</v>
-      </c>
-      <c r="F50">
-        <v>1</v>
-      </c>
-      <c r="G50" s="5">
-        <v>0</v>
+      <c r="F50" s="5">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
       </c>
       <c r="H50" s="5">
-        <v>1</v>
-      </c>
-      <c r="I50" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I50" s="5">
+        <v>1</v>
+      </c>
+      <c r="J50" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B51" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C51" s="5">
         <v>3549</v>
       </c>
-      <c r="C51" s="5">
+      <c r="D51" s="5">
         <v>3701</v>
       </c>
-      <c r="D51" s="6">
+      <c r="E51" s="6">
         <v>105</v>
       </c>
-      <c r="E51" s="5">
-        <v>0</v>
-      </c>
-      <c r="F51">
-        <v>1</v>
-      </c>
-      <c r="G51" s="5">
-        <v>0</v>
+      <c r="F51" s="5">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
       </c>
       <c r="H51" s="5">
-        <v>1</v>
-      </c>
-      <c r="I51" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I51" s="5">
+        <v>1</v>
+      </c>
+      <c r="J51" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B52" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52" s="5">
         <v>4272</v>
       </c>
-      <c r="C52" s="5">
+      <c r="D52" s="5">
         <v>4423</v>
       </c>
-      <c r="D52" s="6">
+      <c r="E52" s="6">
         <v>283</v>
       </c>
-      <c r="E52" s="5">
-        <v>0</v>
-      </c>
-      <c r="F52">
-        <v>1</v>
-      </c>
-      <c r="G52" s="5">
-        <v>0</v>
+      <c r="F52" s="5">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
       </c>
       <c r="H52" s="5">
-        <v>1</v>
-      </c>
-      <c r="I52" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I52" s="5">
+        <v>1</v>
+      </c>
+      <c r="J52" s="5" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>